<commit_message>
31 May to 31 July AWS data cleaned and added
</commit_message>
<xml_diff>
--- a/metadata/IMEI_numbers_station_2021-10-27.xlsx
+++ b/metadata/IMEI_numbers_station_2021-10-27.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10912"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10713"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jason/Dropbox/AWS/test/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jason/Dropbox/AWS/CARRA-TU_GEUS/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CA39143-A2C4-3741-84F4-13570B9D5D9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CB32254-317E-FE47-99BC-E82849D13F33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="800" yWindow="500" windowWidth="33120" windowHeight="16100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11200" yWindow="500" windowWidth="28800" windowHeight="16100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Table 1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="121">
   <si>
     <r>
       <rPr>
@@ -1099,6 +1099,15 @@
   </si>
   <si>
     <t>QAS_U2</t>
+  </si>
+  <si>
+    <t>CP1_2021</t>
+  </si>
+  <si>
+    <t>JAR_U</t>
+  </si>
+  <si>
+    <t>SWC_U</t>
   </si>
 </sst>
 </file>
@@ -1172,7 +1181,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -1215,11 +1224,14 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="7"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="7"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1562,10 +1574,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J48"/>
+  <dimension ref="A1:J51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J22" sqref="J22"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="J52" sqref="J52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1619,10 +1631,10 @@
       <c r="B2" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" s="14"/>
+      <c r="C2" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="16"/>
       <c r="E2" s="6" t="s">
         <v>9</v>
       </c>
@@ -1678,10 +1690,10 @@
       <c r="A4" s="5">
         <v>300234061478500</v>
       </c>
-      <c r="B4" s="16" t="s">
+      <c r="B4" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="16"/>
+      <c r="C4" s="17"/>
       <c r="D4" s="6" t="s">
         <v>8</v>
       </c>
@@ -1740,10 +1752,10 @@
       <c r="A6" s="5">
         <v>300234061295270</v>
       </c>
-      <c r="B6" s="16" t="s">
+      <c r="B6" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="C6" s="16"/>
+      <c r="C6" s="17"/>
       <c r="D6" s="6" t="s">
         <v>8</v>
       </c>
@@ -1802,10 +1814,10 @@
       <c r="A8" s="5">
         <v>300234061165160</v>
       </c>
-      <c r="B8" s="16" t="s">
+      <c r="B8" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="C8" s="16"/>
+      <c r="C8" s="17"/>
       <c r="D8" s="6" t="s">
         <v>8</v>
       </c>
@@ -1864,10 +1876,10 @@
       <c r="A10" s="5">
         <v>300234061627590</v>
       </c>
-      <c r="B10" s="16" t="s">
+      <c r="B10" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="C10" s="16"/>
+      <c r="C10" s="17"/>
       <c r="D10" s="6" t="s">
         <v>8</v>
       </c>
@@ -1926,10 +1938,10 @@
       <c r="A12" s="5">
         <v>300234064126980</v>
       </c>
-      <c r="B12" s="16" t="s">
+      <c r="B12" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="C12" s="16"/>
+      <c r="C12" s="17"/>
       <c r="D12" s="6" t="s">
         <v>8</v>
       </c>
@@ -1988,10 +2000,10 @@
       <c r="A14" s="5">
         <v>300034012437350</v>
       </c>
-      <c r="B14" s="16" t="s">
+      <c r="B14" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="C14" s="16"/>
+      <c r="C14" s="17"/>
       <c r="D14" s="6" t="s">
         <v>8</v>
       </c>
@@ -2050,10 +2062,10 @@
       <c r="A16" s="5">
         <v>300034012776170</v>
       </c>
-      <c r="B16" s="16" t="s">
+      <c r="B16" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="C16" s="16"/>
+      <c r="C16" s="17"/>
       <c r="D16" s="6" t="s">
         <v>8</v>
       </c>
@@ -2112,10 +2124,10 @@
       <c r="A18" s="5">
         <v>300234061218540</v>
       </c>
-      <c r="B18" s="16" t="s">
+      <c r="B18" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="C18" s="16"/>
+      <c r="C18" s="17"/>
       <c r="D18" s="6" t="s">
         <v>8</v>
       </c>
@@ -2174,10 +2186,10 @@
       <c r="A20" s="5">
         <v>300034012930510</v>
       </c>
-      <c r="B20" s="16" t="s">
+      <c r="B20" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="C20" s="16"/>
+      <c r="C20" s="17"/>
       <c r="D20" s="6" t="s">
         <v>8</v>
       </c>
@@ -2236,10 +2248,10 @@
       <c r="A22" s="5">
         <v>300234065156620</v>
       </c>
-      <c r="B22" s="16" t="s">
+      <c r="B22" s="17" t="s">
         <v>49</v>
       </c>
-      <c r="C22" s="16"/>
+      <c r="C22" s="17"/>
       <c r="D22" s="6" t="s">
         <v>8</v>
       </c>
@@ -2298,10 +2310,10 @@
       <c r="A24" s="5">
         <v>300234065158630</v>
       </c>
-      <c r="B24" s="16" t="s">
+      <c r="B24" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="C24" s="16"/>
+      <c r="C24" s="17"/>
       <c r="D24" s="6" t="s">
         <v>8</v>
       </c>
@@ -2360,10 +2372,10 @@
       <c r="A26" s="5">
         <v>300234065157600</v>
       </c>
-      <c r="B26" s="16" t="s">
+      <c r="B26" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="C26" s="16"/>
+      <c r="C26" s="17"/>
       <c r="D26" s="6" t="s">
         <v>8</v>
       </c>
@@ -2421,10 +2433,10 @@
       <c r="A28" s="5">
         <v>300234066313290</v>
       </c>
-      <c r="B28" s="16" t="s">
+      <c r="B28" s="17" t="s">
         <v>61</v>
       </c>
-      <c r="C28" s="16"/>
+      <c r="C28" s="17"/>
       <c r="D28" s="6" t="s">
         <v>8</v>
       </c>
@@ -2483,10 +2495,10 @@
       <c r="A30" s="5">
         <v>300234066318240</v>
       </c>
-      <c r="B30" s="16" t="s">
+      <c r="B30" s="17" t="s">
         <v>65</v>
       </c>
-      <c r="C30" s="16"/>
+      <c r="C30" s="17"/>
       <c r="D30" s="6" t="s">
         <v>8</v>
       </c>
@@ -2544,10 +2556,10 @@
       <c r="A32" s="5">
         <v>300234066319330</v>
       </c>
-      <c r="B32" s="16" t="s">
+      <c r="B32" s="17" t="s">
         <v>69</v>
       </c>
-      <c r="C32" s="16"/>
+      <c r="C32" s="17"/>
       <c r="D32" s="6" t="s">
         <v>8</v>
       </c>
@@ -2606,10 +2618,10 @@
       <c r="A34" s="5">
         <v>300234068626510</v>
       </c>
-      <c r="B34" s="16" t="s">
+      <c r="B34" s="17" t="s">
         <v>73</v>
       </c>
-      <c r="C34" s="16"/>
+      <c r="C34" s="17"/>
       <c r="D34" s="6" t="s">
         <v>8</v>
       </c>
@@ -2668,10 +2680,10 @@
       <c r="A36" s="5">
         <v>300234068420030</v>
       </c>
-      <c r="B36" s="16" t="s">
+      <c r="B36" s="17" t="s">
         <v>77</v>
       </c>
-      <c r="C36" s="16"/>
+      <c r="C36" s="17"/>
       <c r="D36" s="6" t="s">
         <v>8</v>
       </c>
@@ -2730,10 +2742,10 @@
       <c r="A38" s="5">
         <v>300534060523260</v>
       </c>
-      <c r="B38" s="16" t="s">
+      <c r="B38" s="17" t="s">
         <v>103</v>
       </c>
-      <c r="C38" s="16"/>
+      <c r="C38" s="17"/>
       <c r="D38" s="6" t="s">
         <v>8</v>
       </c>
@@ -2792,10 +2804,10 @@
       <c r="A40" s="5">
         <v>300534060520350</v>
       </c>
-      <c r="B40" s="16" t="s">
+      <c r="B40" s="17" t="s">
         <v>84</v>
       </c>
-      <c r="C40" s="16"/>
+      <c r="C40" s="17"/>
       <c r="D40" s="6" t="s">
         <v>8</v>
       </c>
@@ -2852,10 +2864,10 @@
       <c r="A42" s="5">
         <v>300534062412950</v>
       </c>
-      <c r="B42" s="16" t="s">
+      <c r="B42" s="17" t="s">
         <v>88</v>
       </c>
-      <c r="C42" s="16"/>
+      <c r="C42" s="17"/>
       <c r="D42" s="6" t="s">
         <v>8</v>
       </c>
@@ -2899,7 +2911,7 @@
         <v>91</v>
       </c>
       <c r="H43" s="11" t="s">
-        <v>109</v>
+        <v>118</v>
       </c>
       <c r="I43">
         <v>1</v>
@@ -2912,10 +2924,10 @@
       <c r="A44" s="5">
         <v>300534062416350</v>
       </c>
-      <c r="B44" s="16" t="s">
+      <c r="B44" s="17" t="s">
         <v>92</v>
       </c>
-      <c r="C44" s="16"/>
+      <c r="C44" s="17"/>
       <c r="D44" s="6" t="s">
         <v>8</v>
       </c>
@@ -2972,10 +2984,10 @@
       <c r="A46" s="5">
         <v>300534062417910</v>
       </c>
-      <c r="B46" s="16" t="s">
+      <c r="B46" s="17" t="s">
         <v>95</v>
       </c>
-      <c r="C46" s="16"/>
+      <c r="C46" s="17"/>
       <c r="D46" s="6" t="s">
         <v>8</v>
       </c>
@@ -3033,10 +3045,10 @@
       <c r="A48" s="5">
         <v>300534060529320</v>
       </c>
-      <c r="B48" s="16" t="s">
+      <c r="B48" s="17" t="s">
         <v>99</v>
       </c>
-      <c r="C48" s="16"/>
+      <c r="C48" s="17"/>
       <c r="D48" s="6" t="s">
         <v>8</v>
       </c>
@@ -3060,8 +3072,74 @@
         <v>102</v>
       </c>
     </row>
+    <row r="49" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A49" s="8">
+        <v>300534062024750</v>
+      </c>
+      <c r="B49" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="C49" s="15"/>
+      <c r="D49" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="E49" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="F49" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="G49" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="H49" s="11" t="s">
+        <v>109</v>
+      </c>
+      <c r="I49">
+        <v>1</v>
+      </c>
+      <c r="J49" s="12" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A50">
+        <v>300534063816770</v>
+      </c>
+      <c r="B50" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="H50" t="str">
+        <f>B50</f>
+        <v>SWC_U</v>
+      </c>
+      <c r="I50">
+        <v>1</v>
+      </c>
+      <c r="J50" s="12" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A51">
+        <v>300534063814490</v>
+      </c>
+      <c r="B51" t="s">
+        <v>119</v>
+      </c>
+      <c r="H51" t="str">
+        <f>B51</f>
+        <v>JAR_U</v>
+      </c>
+      <c r="I51">
+        <v>1</v>
+      </c>
+      <c r="J51" s="12" t="s">
+        <v>114</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="47">
+  <mergeCells count="48">
     <mergeCell ref="B45:C45"/>
     <mergeCell ref="B46:C46"/>
     <mergeCell ref="B47:C47"/>
@@ -3094,21 +3172,22 @@
     <mergeCell ref="B19:C19"/>
     <mergeCell ref="B20:C20"/>
     <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B49:C49"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B11:C11"/>
     <mergeCell ref="B12:C12"/>
     <mergeCell ref="B13:C13"/>
     <mergeCell ref="B14:C14"/>
     <mergeCell ref="B15:C15"/>
     <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B6:C6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
fix JAR, SWC, CP1, NSE, SDM, added QAS_U2, CP1_2021
</commit_message>
<xml_diff>
--- a/metadata/IMEI_numbers_station_2021-10-27.xlsx
+++ b/metadata/IMEI_numbers_station_2021-10-27.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jason/Dropbox/AWS/CARRA-TU_GEUS/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CB32254-317E-FE47-99BC-E82849D13F33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABE7E2CE-28BC-964B-8755-637EC8DBF52E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11200" yWindow="500" windowWidth="28800" windowHeight="16100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Table 1" sheetId="1" r:id="rId1"/>
@@ -1231,10 +1231,10 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="7"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="7"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1576,8 +1576,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="J52" sqref="J52"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1631,10 +1631,10 @@
       <c r="B2" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" s="16"/>
+      <c r="C2" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="17"/>
       <c r="E2" s="6" t="s">
         <v>9</v>
       </c>
@@ -1690,10 +1690,10 @@
       <c r="A4" s="5">
         <v>300234061478500</v>
       </c>
-      <c r="B4" s="17" t="s">
+      <c r="B4" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="17"/>
+      <c r="C4" s="16"/>
       <c r="D4" s="6" t="s">
         <v>8</v>
       </c>
@@ -1752,10 +1752,10 @@
       <c r="A6" s="5">
         <v>300234061295270</v>
       </c>
-      <c r="B6" s="17" t="s">
+      <c r="B6" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="C6" s="17"/>
+      <c r="C6" s="16"/>
       <c r="D6" s="6" t="s">
         <v>8</v>
       </c>
@@ -1814,10 +1814,10 @@
       <c r="A8" s="5">
         <v>300234061165160</v>
       </c>
-      <c r="B8" s="17" t="s">
+      <c r="B8" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="C8" s="17"/>
+      <c r="C8" s="16"/>
       <c r="D8" s="6" t="s">
         <v>8</v>
       </c>
@@ -1876,10 +1876,10 @@
       <c r="A10" s="5">
         <v>300234061627590</v>
       </c>
-      <c r="B10" s="17" t="s">
+      <c r="B10" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="C10" s="17"/>
+      <c r="C10" s="16"/>
       <c r="D10" s="6" t="s">
         <v>8</v>
       </c>
@@ -1938,10 +1938,10 @@
       <c r="A12" s="5">
         <v>300234064126980</v>
       </c>
-      <c r="B12" s="17" t="s">
+      <c r="B12" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="C12" s="17"/>
+      <c r="C12" s="16"/>
       <c r="D12" s="6" t="s">
         <v>8</v>
       </c>
@@ -2000,10 +2000,10 @@
       <c r="A14" s="5">
         <v>300034012437350</v>
       </c>
-      <c r="B14" s="17" t="s">
+      <c r="B14" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="C14" s="17"/>
+      <c r="C14" s="16"/>
       <c r="D14" s="6" t="s">
         <v>8</v>
       </c>
@@ -2062,10 +2062,10 @@
       <c r="A16" s="5">
         <v>300034012776170</v>
       </c>
-      <c r="B16" s="17" t="s">
+      <c r="B16" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="C16" s="17"/>
+      <c r="C16" s="16"/>
       <c r="D16" s="6" t="s">
         <v>8</v>
       </c>
@@ -2124,10 +2124,10 @@
       <c r="A18" s="5">
         <v>300234061218540</v>
       </c>
-      <c r="B18" s="17" t="s">
+      <c r="B18" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="C18" s="17"/>
+      <c r="C18" s="16"/>
       <c r="D18" s="6" t="s">
         <v>8</v>
       </c>
@@ -2186,10 +2186,10 @@
       <c r="A20" s="5">
         <v>300034012930510</v>
       </c>
-      <c r="B20" s="17" t="s">
+      <c r="B20" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="C20" s="17"/>
+      <c r="C20" s="16"/>
       <c r="D20" s="6" t="s">
         <v>8</v>
       </c>
@@ -2248,10 +2248,10 @@
       <c r="A22" s="5">
         <v>300234065156620</v>
       </c>
-      <c r="B22" s="17" t="s">
+      <c r="B22" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="C22" s="17"/>
+      <c r="C22" s="16"/>
       <c r="D22" s="6" t="s">
         <v>8</v>
       </c>
@@ -2310,10 +2310,10 @@
       <c r="A24" s="5">
         <v>300234065158630</v>
       </c>
-      <c r="B24" s="17" t="s">
+      <c r="B24" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="C24" s="17"/>
+      <c r="C24" s="16"/>
       <c r="D24" s="6" t="s">
         <v>8</v>
       </c>
@@ -2372,10 +2372,10 @@
       <c r="A26" s="5">
         <v>300234065157600</v>
       </c>
-      <c r="B26" s="17" t="s">
+      <c r="B26" s="16" t="s">
         <v>57</v>
       </c>
-      <c r="C26" s="17"/>
+      <c r="C26" s="16"/>
       <c r="D26" s="6" t="s">
         <v>8</v>
       </c>
@@ -2426,17 +2426,17 @@
         <v>1</v>
       </c>
       <c r="J27" s="13" t="s">
-        <v>115</v>
+        <v>102</v>
       </c>
     </row>
     <row r="28" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="5">
         <v>300234066313290</v>
       </c>
-      <c r="B28" s="17" t="s">
+      <c r="B28" s="16" t="s">
         <v>61</v>
       </c>
-      <c r="C28" s="17"/>
+      <c r="C28" s="16"/>
       <c r="D28" s="6" t="s">
         <v>8</v>
       </c>
@@ -2495,10 +2495,10 @@
       <c r="A30" s="5">
         <v>300234066318240</v>
       </c>
-      <c r="B30" s="17" t="s">
+      <c r="B30" s="16" t="s">
         <v>65</v>
       </c>
-      <c r="C30" s="17"/>
+      <c r="C30" s="16"/>
       <c r="D30" s="6" t="s">
         <v>8</v>
       </c>
@@ -2556,10 +2556,10 @@
       <c r="A32" s="5">
         <v>300234066319330</v>
       </c>
-      <c r="B32" s="17" t="s">
+      <c r="B32" s="16" t="s">
         <v>69</v>
       </c>
-      <c r="C32" s="17"/>
+      <c r="C32" s="16"/>
       <c r="D32" s="6" t="s">
         <v>8</v>
       </c>
@@ -2618,10 +2618,10 @@
       <c r="A34" s="5">
         <v>300234068626510</v>
       </c>
-      <c r="B34" s="17" t="s">
+      <c r="B34" s="16" t="s">
         <v>73</v>
       </c>
-      <c r="C34" s="17"/>
+      <c r="C34" s="16"/>
       <c r="D34" s="6" t="s">
         <v>8</v>
       </c>
@@ -2680,10 +2680,10 @@
       <c r="A36" s="5">
         <v>300234068420030</v>
       </c>
-      <c r="B36" s="17" t="s">
+      <c r="B36" s="16" t="s">
         <v>77</v>
       </c>
-      <c r="C36" s="17"/>
+      <c r="C36" s="16"/>
       <c r="D36" s="6" t="s">
         <v>8</v>
       </c>
@@ -2742,10 +2742,10 @@
       <c r="A38" s="5">
         <v>300534060523260</v>
       </c>
-      <c r="B38" s="17" t="s">
+      <c r="B38" s="16" t="s">
         <v>103</v>
       </c>
-      <c r="C38" s="17"/>
+      <c r="C38" s="16"/>
       <c r="D38" s="6" t="s">
         <v>8</v>
       </c>
@@ -2804,10 +2804,10 @@
       <c r="A40" s="5">
         <v>300534060520350</v>
       </c>
-      <c r="B40" s="17" t="s">
+      <c r="B40" s="16" t="s">
         <v>84</v>
       </c>
-      <c r="C40" s="17"/>
+      <c r="C40" s="16"/>
       <c r="D40" s="6" t="s">
         <v>8</v>
       </c>
@@ -2864,10 +2864,10 @@
       <c r="A42" s="5">
         <v>300534062412950</v>
       </c>
-      <c r="B42" s="17" t="s">
+      <c r="B42" s="16" t="s">
         <v>88</v>
       </c>
-      <c r="C42" s="17"/>
+      <c r="C42" s="16"/>
       <c r="D42" s="6" t="s">
         <v>8</v>
       </c>
@@ -2924,10 +2924,10 @@
       <c r="A44" s="5">
         <v>300534062416350</v>
       </c>
-      <c r="B44" s="17" t="s">
+      <c r="B44" s="16" t="s">
         <v>92</v>
       </c>
-      <c r="C44" s="17"/>
+      <c r="C44" s="16"/>
       <c r="D44" s="6" t="s">
         <v>8</v>
       </c>
@@ -2984,10 +2984,10 @@
       <c r="A46" s="5">
         <v>300534062417910</v>
       </c>
-      <c r="B46" s="17" t="s">
+      <c r="B46" s="16" t="s">
         <v>95</v>
       </c>
-      <c r="C46" s="17"/>
+      <c r="C46" s="16"/>
       <c r="D46" s="6" t="s">
         <v>8</v>
       </c>
@@ -3045,10 +3045,10 @@
       <c r="A48" s="5">
         <v>300534060529320</v>
       </c>
-      <c r="B48" s="17" t="s">
+      <c r="B48" s="16" t="s">
         <v>99</v>
       </c>
-      <c r="C48" s="17"/>
+      <c r="C48" s="16"/>
       <c r="D48" s="6" t="s">
         <v>8</v>
       </c>
@@ -3140,38 +3140,6 @@
     </row>
   </sheetData>
   <mergeCells count="48">
-    <mergeCell ref="B45:C45"/>
-    <mergeCell ref="B46:C46"/>
-    <mergeCell ref="B47:C47"/>
-    <mergeCell ref="B48:C48"/>
-    <mergeCell ref="B40:C40"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="B43:C43"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="B35:C35"/>
-    <mergeCell ref="B36:C36"/>
-    <mergeCell ref="B37:C37"/>
-    <mergeCell ref="B38:C38"/>
-    <mergeCell ref="B39:C39"/>
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="B33:C33"/>
-    <mergeCell ref="B34:C34"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="B21:C21"/>
     <mergeCell ref="B49:C49"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="B3:C3"/>
@@ -3188,6 +3156,38 @@
     <mergeCell ref="B14:C14"/>
     <mergeCell ref="B15:C15"/>
     <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="B37:C37"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="B39:C39"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="B46:C46"/>
+    <mergeCell ref="B47:C47"/>
+    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="B40:C40"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="B43:C43"/>
+    <mergeCell ref="B44:C44"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
WSL GC-Net and further work
</commit_message>
<xml_diff>
--- a/metadata/IMEI_numbers_station_2021-10-27.xlsx
+++ b/metadata/IMEI_numbers_station_2021-10-27.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10911"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jason/Dropbox/AWS/CARRA-TU_GEUS/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABE7E2CE-28BC-964B-8755-637EC8DBF52E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9CFFCBD-4DE2-0D44-9E5A-D90FC501DCC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="31660" windowHeight="20840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Table 1" sheetId="1" r:id="rId1"/>
@@ -20,9 +20,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
@@ -31,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="119">
   <si>
     <r>
       <rPr>
@@ -816,16 +814,6 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>NUK_U V3</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
       <t>2020-01-16 13:22:58</t>
     </r>
   </si>
@@ -886,16 +874,6 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>JAR1</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
       <t>2020-09-24 12:11:42</t>
     </r>
   </si>
@@ -906,16 +884,6 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>GCNET SADDLE</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
       <t>2021-06-02 13:19:56</t>
     </r>
   </si>
@@ -1108,6 +1076,9 @@
   </si>
   <si>
     <t>SWC_U</t>
+  </si>
+  <si>
+    <t>NUK_Uv3</t>
   </si>
 </sst>
 </file>
@@ -1231,10 +1202,10 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="7"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="7"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1577,7 +1548,7 @@
   <dimension ref="A1:J51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M11" sqref="M11"/>
+      <selection activeCell="B37" sqref="B37:C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1615,13 +1586,13 @@
         <v>6</v>
       </c>
       <c r="H1" s="11" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="I1" s="12" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="J1" s="12" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -1631,10 +1602,10 @@
       <c r="B2" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" s="17"/>
+      <c r="C2" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="16"/>
       <c r="E2" s="6" t="s">
         <v>9</v>
       </c>
@@ -1652,7 +1623,7 @@
         <v>1</v>
       </c>
       <c r="J2" s="12" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -1683,17 +1654,17 @@
         <v>1</v>
       </c>
       <c r="J3" s="12" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="5">
         <v>300234061478500</v>
       </c>
-      <c r="B4" s="16" t="s">
+      <c r="B4" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="16"/>
+      <c r="C4" s="17"/>
       <c r="D4" s="6" t="s">
         <v>8</v>
       </c>
@@ -1714,7 +1685,7 @@
         <v>1</v>
       </c>
       <c r="J4" s="12" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.15">
@@ -1745,17 +1716,17 @@
         <v>1</v>
       </c>
       <c r="J5" s="12" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="5">
         <v>300234061295270</v>
       </c>
-      <c r="B6" s="16" t="s">
+      <c r="B6" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="C6" s="16"/>
+      <c r="C6" s="17"/>
       <c r="D6" s="6" t="s">
         <v>8</v>
       </c>
@@ -1776,7 +1747,7 @@
         <v>1</v>
       </c>
       <c r="J6" s="12" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -1807,17 +1778,17 @@
         <v>1</v>
       </c>
       <c r="J7" s="13" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="5">
         <v>300234061165160</v>
       </c>
-      <c r="B8" s="16" t="s">
+      <c r="B8" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="C8" s="16"/>
+      <c r="C8" s="17"/>
       <c r="D8" s="6" t="s">
         <v>8</v>
       </c>
@@ -1838,7 +1809,7 @@
         <v>1</v>
       </c>
       <c r="J8" s="12" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.15">
@@ -1869,17 +1840,17 @@
         <v>1</v>
       </c>
       <c r="J9" s="12" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="5">
         <v>300234061627590</v>
       </c>
-      <c r="B10" s="16" t="s">
+      <c r="B10" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="C10" s="16"/>
+      <c r="C10" s="17"/>
       <c r="D10" s="6" t="s">
         <v>8</v>
       </c>
@@ -1900,7 +1871,7 @@
         <v>1</v>
       </c>
       <c r="J10" s="12" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.15">
@@ -1931,17 +1902,17 @@
         <v>1</v>
       </c>
       <c r="J11" s="13" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="5">
         <v>300234064126980</v>
       </c>
-      <c r="B12" s="16" t="s">
+      <c r="B12" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="C12" s="16"/>
+      <c r="C12" s="17"/>
       <c r="D12" s="6" t="s">
         <v>8</v>
       </c>
@@ -1962,7 +1933,7 @@
         <v>1</v>
       </c>
       <c r="J12" s="12" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.15">
@@ -1993,17 +1964,17 @@
         <v>1</v>
       </c>
       <c r="J13" s="13" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="5">
         <v>300034012437350</v>
       </c>
-      <c r="B14" s="16" t="s">
+      <c r="B14" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="C14" s="16"/>
+      <c r="C14" s="17"/>
       <c r="D14" s="6" t="s">
         <v>8</v>
       </c>
@@ -2024,7 +1995,7 @@
         <v>1</v>
       </c>
       <c r="J14" s="13" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.15">
@@ -2055,17 +2026,17 @@
         <v>1</v>
       </c>
       <c r="J15" s="12" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="5">
         <v>300034012776170</v>
       </c>
-      <c r="B16" s="16" t="s">
+      <c r="B16" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="C16" s="16"/>
+      <c r="C16" s="17"/>
       <c r="D16" s="6" t="s">
         <v>8</v>
       </c>
@@ -2086,7 +2057,7 @@
         <v>1</v>
       </c>
       <c r="J16" s="12" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.15">
@@ -2117,17 +2088,17 @@
         <v>1</v>
       </c>
       <c r="J17" s="13" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="5">
         <v>300234061218540</v>
       </c>
-      <c r="B18" s="16" t="s">
+      <c r="B18" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="C18" s="16"/>
+      <c r="C18" s="17"/>
       <c r="D18" s="6" t="s">
         <v>8</v>
       </c>
@@ -2148,7 +2119,7 @@
         <v>1</v>
       </c>
       <c r="J18" s="13" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
     </row>
     <row r="19" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.15">
@@ -2179,17 +2150,17 @@
         <v>1</v>
       </c>
       <c r="J19" s="12" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="20" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="5">
         <v>300034012930510</v>
       </c>
-      <c r="B20" s="16" t="s">
+      <c r="B20" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="C20" s="16"/>
+      <c r="C20" s="17"/>
       <c r="D20" s="6" t="s">
         <v>8</v>
       </c>
@@ -2210,7 +2181,7 @@
         <v>1</v>
       </c>
       <c r="J20" s="12" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="21" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -2241,17 +2212,17 @@
         <v>1</v>
       </c>
       <c r="J21" s="13" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="22" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="5">
         <v>300234065156620</v>
       </c>
-      <c r="B22" s="16" t="s">
+      <c r="B22" s="17" t="s">
         <v>49</v>
       </c>
-      <c r="C22" s="16"/>
+      <c r="C22" s="17"/>
       <c r="D22" s="6" t="s">
         <v>8</v>
       </c>
@@ -2272,7 +2243,7 @@
         <v>1</v>
       </c>
       <c r="J22" s="13" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
     </row>
     <row r="23" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.15">
@@ -2303,17 +2274,17 @@
         <v>1</v>
       </c>
       <c r="J23" s="12" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="24" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="5">
         <v>300234065158630</v>
       </c>
-      <c r="B24" s="16" t="s">
+      <c r="B24" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="C24" s="16"/>
+      <c r="C24" s="17"/>
       <c r="D24" s="6" t="s">
         <v>8</v>
       </c>
@@ -2334,7 +2305,7 @@
         <v>1</v>
       </c>
       <c r="J24" s="13" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
     </row>
     <row r="25" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -2365,17 +2336,17 @@
         <v>1</v>
       </c>
       <c r="J25" s="12" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="26" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="5">
         <v>300234065157600</v>
       </c>
-      <c r="B26" s="16" t="s">
+      <c r="B26" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="C26" s="16"/>
+      <c r="C26" s="17"/>
       <c r="D26" s="6" t="s">
         <v>8</v>
       </c>
@@ -2396,7 +2367,7 @@
         <v>1</v>
       </c>
       <c r="J26" s="12" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="27" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.15">
@@ -2420,23 +2391,23 @@
         <v>60</v>
       </c>
       <c r="H27" s="11" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="I27">
         <v>1</v>
       </c>
       <c r="J27" s="13" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="28" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="5">
         <v>300234066313290</v>
       </c>
-      <c r="B28" s="16" t="s">
+      <c r="B28" s="17" t="s">
         <v>61</v>
       </c>
-      <c r="C28" s="16"/>
+      <c r="C28" s="17"/>
       <c r="D28" s="6" t="s">
         <v>8</v>
       </c>
@@ -2457,7 +2428,7 @@
         <v>1</v>
       </c>
       <c r="J28" s="13" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
     </row>
     <row r="29" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.15">
@@ -2488,17 +2459,17 @@
         <v>1</v>
       </c>
       <c r="J29" s="12" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="30" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="5">
         <v>300234066318240</v>
       </c>
-      <c r="B30" s="16" t="s">
+      <c r="B30" s="17" t="s">
         <v>65</v>
       </c>
-      <c r="C30" s="16"/>
+      <c r="C30" s="17"/>
       <c r="D30" s="6" t="s">
         <v>8</v>
       </c>
@@ -2512,13 +2483,13 @@
         <v>66</v>
       </c>
       <c r="H30" s="11" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="I30">
         <v>1</v>
       </c>
       <c r="J30" s="12" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="31" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.15">
@@ -2549,17 +2520,17 @@
         <v>1</v>
       </c>
       <c r="J31" s="12" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="32" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="5">
         <v>300234066319330</v>
       </c>
-      <c r="B32" s="16" t="s">
+      <c r="B32" s="17" t="s">
         <v>69</v>
       </c>
-      <c r="C32" s="16"/>
+      <c r="C32" s="17"/>
       <c r="D32" s="6" t="s">
         <v>8</v>
       </c>
@@ -2580,7 +2551,7 @@
         <v>1</v>
       </c>
       <c r="J32" s="12" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="33" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.15">
@@ -2611,17 +2582,17 @@
         <v>1</v>
       </c>
       <c r="J33" s="13" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
     </row>
     <row r="34" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A34" s="5">
         <v>300234068626510</v>
       </c>
-      <c r="B34" s="16" t="s">
+      <c r="B34" s="17" t="s">
         <v>73</v>
       </c>
-      <c r="C34" s="16"/>
+      <c r="C34" s="17"/>
       <c r="D34" s="6" t="s">
         <v>8</v>
       </c>
@@ -2642,7 +2613,7 @@
         <v>1</v>
       </c>
       <c r="J34" s="13" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
     </row>
     <row r="35" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.15">
@@ -2673,38 +2644,38 @@
         <v>1</v>
       </c>
       <c r="J35" s="13" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
     </row>
     <row r="36" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A36" s="5">
         <v>300234068420030</v>
       </c>
-      <c r="B36" s="16" t="s">
+      <c r="B36" s="17" t="s">
+        <v>118</v>
+      </c>
+      <c r="C36" s="17"/>
+      <c r="D36" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E36" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F36" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="G36" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="C36" s="16"/>
-      <c r="D36" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E36" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="F36" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="G36" s="7" t="s">
-        <v>78</v>
-      </c>
       <c r="H36" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>NUK_U V3</v>
+        <v>NUK_Uv3</v>
       </c>
       <c r="I36">
         <v>1</v>
       </c>
       <c r="J36" s="13" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
     </row>
     <row r="37" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -2712,7 +2683,7 @@
         <v>300234068423000</v>
       </c>
       <c r="B37" s="15" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C37" s="15"/>
       <c r="D37" s="9" t="s">
@@ -2725,7 +2696,7 @@
         <v>10</v>
       </c>
       <c r="G37" s="10" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H37" s="4" t="str">
         <f t="shared" si="0"/>
@@ -2735,17 +2706,17 @@
         <v>1</v>
       </c>
       <c r="J37" s="13" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
     </row>
     <row r="38" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A38" s="5">
         <v>300534060523260</v>
       </c>
-      <c r="B38" s="16" t="s">
-        <v>103</v>
-      </c>
-      <c r="C38" s="16"/>
+      <c r="B38" s="17" t="s">
+        <v>100</v>
+      </c>
+      <c r="C38" s="17"/>
       <c r="D38" s="6" t="s">
         <v>8</v>
       </c>
@@ -2756,7 +2727,7 @@
         <v>10</v>
       </c>
       <c r="G38" s="7" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H38" s="4" t="str">
         <f t="shared" si="0"/>
@@ -2766,7 +2737,7 @@
         <v>1</v>
       </c>
       <c r="J38" s="13" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
     </row>
     <row r="39" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.15">
@@ -2774,7 +2745,7 @@
         <v>300534060524310</v>
       </c>
       <c r="B39" s="15" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C39" s="15"/>
       <c r="D39" s="9" t="s">
@@ -2787,7 +2758,7 @@
         <v>10</v>
       </c>
       <c r="G39" s="10" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="H39" s="4" t="str">
         <f t="shared" si="0"/>
@@ -2797,17 +2768,17 @@
         <v>1</v>
       </c>
       <c r="J39" s="12" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="40" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A40" s="5">
         <v>300534060520350</v>
       </c>
-      <c r="B40" s="16" t="s">
-        <v>84</v>
-      </c>
-      <c r="C40" s="16"/>
+      <c r="B40" s="17" t="s">
+        <v>109</v>
+      </c>
+      <c r="C40" s="17"/>
       <c r="D40" s="6" t="s">
         <v>8</v>
       </c>
@@ -2818,16 +2789,16 @@
         <v>10</v>
       </c>
       <c r="G40" s="7" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="H40" s="11" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="I40">
         <v>1</v>
       </c>
       <c r="J40" s="12" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="41" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -2835,7 +2806,7 @@
         <v>300534062415410</v>
       </c>
       <c r="B41" s="15" t="s">
-        <v>86</v>
+        <v>108</v>
       </c>
       <c r="C41" s="15"/>
       <c r="D41" s="9" t="s">
@@ -2848,26 +2819,26 @@
         <v>10</v>
       </c>
       <c r="G41" s="10" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="H41" s="11" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="I41">
         <v>1</v>
       </c>
       <c r="J41" s="13" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
     </row>
     <row r="42" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A42" s="5">
         <v>300534062412950</v>
       </c>
-      <c r="B42" s="16" t="s">
-        <v>88</v>
-      </c>
-      <c r="C42" s="16"/>
+      <c r="B42" s="17" t="s">
+        <v>85</v>
+      </c>
+      <c r="C42" s="17"/>
       <c r="D42" s="6" t="s">
         <v>8</v>
       </c>
@@ -2878,16 +2849,16 @@
         <v>10</v>
       </c>
       <c r="G42" s="7" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="H42" s="11" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="I42">
         <v>1</v>
       </c>
       <c r="J42" s="12" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="43" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.15">
@@ -2895,7 +2866,7 @@
         <v>300534062418810</v>
       </c>
       <c r="B43" s="15" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C43" s="15"/>
       <c r="D43" s="9" t="s">
@@ -2908,26 +2879,26 @@
         <v>10</v>
       </c>
       <c r="G43" s="10" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="H43" s="11" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="I43">
         <v>1</v>
       </c>
       <c r="J43" s="12" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="44" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A44" s="5">
         <v>300534062416350</v>
       </c>
-      <c r="B44" s="16" t="s">
-        <v>92</v>
-      </c>
-      <c r="C44" s="16"/>
+      <c r="B44" s="17" t="s">
+        <v>89</v>
+      </c>
+      <c r="C44" s="17"/>
       <c r="D44" s="6" t="s">
         <v>8</v>
       </c>
@@ -2938,16 +2909,16 @@
         <v>10</v>
       </c>
       <c r="G44" s="7" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="H44" s="11" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="I44">
         <v>1</v>
       </c>
       <c r="J44" s="12" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="45" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -2955,7 +2926,7 @@
         <v>300534062419950</v>
       </c>
       <c r="B45" s="15" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C45" s="15"/>
       <c r="D45" s="9" t="s">
@@ -2968,26 +2939,26 @@
         <v>10</v>
       </c>
       <c r="G45" s="10" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="H45" s="11" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="I45">
         <v>1</v>
       </c>
       <c r="J45" s="12" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="46" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A46" s="5">
         <v>300534062417910</v>
       </c>
-      <c r="B46" s="16" t="s">
-        <v>95</v>
-      </c>
-      <c r="C46" s="16"/>
+      <c r="B46" s="17" t="s">
+        <v>92</v>
+      </c>
+      <c r="C46" s="17"/>
       <c r="D46" s="6" t="s">
         <v>8</v>
       </c>
@@ -2998,7 +2969,7 @@
         <v>10</v>
       </c>
       <c r="G46" s="7" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="H46" s="4" t="str">
         <f t="shared" si="0"/>
@@ -3008,7 +2979,7 @@
         <v>1</v>
       </c>
       <c r="J46" s="12" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="47" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.15">
@@ -3016,7 +2987,7 @@
         <v>300534060529220</v>
       </c>
       <c r="B47" s="15" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C47" s="15"/>
       <c r="D47" s="9" t="s">
@@ -3029,47 +3000,47 @@
         <v>10</v>
       </c>
       <c r="G47" s="10" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="H47" s="11" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="I47">
         <v>1</v>
       </c>
       <c r="J47" s="12" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="48" spans="1:10" ht="15.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="5">
         <v>300534060529320</v>
       </c>
-      <c r="B48" s="16" t="s">
+      <c r="B48" s="17" t="s">
+        <v>96</v>
+      </c>
+      <c r="C48" s="17"/>
+      <c r="D48" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E48" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F48" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="G48" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="H48" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>GEUS</v>
+      </c>
+      <c r="I48">
+        <v>1</v>
+      </c>
+      <c r="J48" s="12" t="s">
         <v>99</v>
-      </c>
-      <c r="C48" s="16"/>
-      <c r="D48" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E48" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="F48" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="G48" s="7" t="s">
-        <v>100</v>
-      </c>
-      <c r="H48" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v>GEUS</v>
-      </c>
-      <c r="I48">
-        <v>1</v>
-      </c>
-      <c r="J48" s="12" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="49" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.15">
@@ -3077,7 +3048,7 @@
         <v>300534062024750</v>
       </c>
       <c r="B49" s="15" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C49" s="15"/>
       <c r="D49" s="14" t="s">
@@ -3090,16 +3061,16 @@
         <v>10</v>
       </c>
       <c r="G49" s="10" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="H49" s="11" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="I49">
         <v>1</v>
       </c>
       <c r="J49" s="12" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.15">
@@ -3107,7 +3078,7 @@
         <v>300534063816770</v>
       </c>
       <c r="B50" s="12" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="H50" t="str">
         <f>B50</f>
@@ -3117,7 +3088,7 @@
         <v>1</v>
       </c>
       <c r="J50" s="12" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.15">
@@ -3125,7 +3096,7 @@
         <v>300534063814490</v>
       </c>
       <c r="B51" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="H51" t="str">
         <f>B51</f>
@@ -3135,11 +3106,43 @@
         <v>1</v>
       </c>
       <c r="J51" s="12" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="48">
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="B46:C46"/>
+    <mergeCell ref="B47:C47"/>
+    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="B40:C40"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="B43:C43"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="B37:C37"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="B39:C39"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B21:C21"/>
     <mergeCell ref="B49:C49"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="B3:C3"/>
@@ -3156,38 +3159,6 @@
     <mergeCell ref="B14:C14"/>
     <mergeCell ref="B15:C15"/>
     <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="B33:C33"/>
-    <mergeCell ref="B34:C34"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="B35:C35"/>
-    <mergeCell ref="B36:C36"/>
-    <mergeCell ref="B37:C37"/>
-    <mergeCell ref="B38:C38"/>
-    <mergeCell ref="B39:C39"/>
-    <mergeCell ref="B45:C45"/>
-    <mergeCell ref="B46:C46"/>
-    <mergeCell ref="B47:C47"/>
-    <mergeCell ref="B48:C48"/>
-    <mergeCell ref="B40:C40"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="B43:C43"/>
-    <mergeCell ref="B44:C44"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>